<commit_message>
Confirmed I have all the latest cards and fixed small issues
</commit_message>
<xml_diff>
--- a/Village_Card_Game_Final_July_2022/All Template Assets/Village Card Game Cards v1.3.xlsx
+++ b/Village_Card_Game_Final_July_2022/All Template Assets/Village Card Game Cards v1.3.xlsx
@@ -350,8 +350,7 @@
     <t>20</t>
   </si>
   <si>
-    <t>Destroy one illegal business. Its owner loses twice that business’ cashflow in reparations. Up to
-$200,000. This effect may not be prevented.</t>
+    <t>Destroy one illegal business. Its owner loses twice that business’ cashflow in reparations. Up to $200k. This effect may not be prevented.</t>
   </si>
   <si>
     <t>Media Promote Education</t>
@@ -490,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -513,6 +512,9 @@
     <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2738,7 +2740,7 @@
       <c r="E14" s="3">
         <v>10.0</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="14" t="s">
         <v>107</v>
       </c>
       <c r="G14" s="11" t="str">
@@ -5023,10 +5025,10 @@
       <c r="F1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -5053,10 +5055,10 @@
       <c r="F2" s="1">
         <v>0.0</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="15">
         <v>0.0</v>
       </c>
-      <c r="H2" s="14"/>
+      <c r="H2" s="15"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4" t="s">
         <v>117</v>
@@ -5076,10 +5078,10 @@
       <c r="F3" s="1">
         <v>0.0</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="15">
         <v>0.0</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="2"/>
       <c r="J3" s="4" t="s">
         <v>119</v>
@@ -5099,10 +5101,10 @@
       <c r="F4" s="1">
         <v>0.0</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="15">
         <v>0.0</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="2"/>
       <c r="J4" s="4" t="s">
         <v>121</v>

</xml_diff>